<commit_message>
Trained BERTissimo (BERT large)
</commit_message>
<xml_diff>
--- a/data/current_best_models.xlsx
+++ b/data/current_best_models.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jack-\Documents\University\Project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9C03CB90-FC55-49A1-BF70-1E3D3699C1F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{692322F4-BFEF-461A-A174-F94BE863BB73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="8490" windowWidth="29040" windowHeight="15840" xr2:uid="{419ADDD1-D059-4EA2-8760-65C135198D45}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Model Name</t>
   </si>
@@ -66,9 +66,6 @@
     <t>LSTM + Attention + BERT</t>
   </si>
   <si>
-    <t>LSTM + Attention + Bert + Side information (Reading)</t>
-  </si>
-  <si>
     <t>CNN + Glove</t>
   </si>
   <si>
@@ -76,6 +73,24 @@
   </si>
   <si>
     <t>RNN + Glove</t>
+  </si>
+  <si>
+    <t>LSTM + Attention + BERT + Side information (Reading)</t>
+  </si>
+  <si>
+    <t>LSTM + Attention + BERT + Normalised Side Information (Reading)</t>
+  </si>
+  <si>
+    <t>LSTM + Attention + BERT +  Pretrained Side Information (Reading)</t>
+  </si>
+  <si>
+    <t>LSTM + Attention + BERT +  Average Layer Side Information (Reading)</t>
+  </si>
+  <si>
+    <t>LSTM + Attention + BERT + Normalised Side Information (Lexical)</t>
+  </si>
+  <si>
+    <t>LSTM + Attention + BERT + Normalised Side Information (Lexical + Human Generated Labels)</t>
   </si>
 </sst>
 </file>
@@ -83,8 +98,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="0.00000"/>
-    <numFmt numFmtId="169" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -244,59 +259,58 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="11">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <family val="2"/>
-      </font>
-      <numFmt numFmtId="168" formatCode="0.00000"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -314,9 +328,9 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="168" formatCode="0.00000"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <numFmt numFmtId="164" formatCode="0.00000"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
           <color rgb="FF000000"/>
         </left>
@@ -325,6 +339,12 @@
         </right>
         <top/>
         <bottom/>
+        <vertical style="medium">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="medium">
+          <color rgb="FF000000"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -344,9 +364,9 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="169" formatCode="0.0000"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <numFmt numFmtId="165" formatCode="0.0000"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
           <color rgb="FF000000"/>
         </left>
@@ -357,6 +377,12 @@
         <bottom style="medium">
           <color rgb="FF000000"/>
         </bottom>
+        <vertical style="medium">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="medium">
+          <color rgb="FF000000"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -376,9 +402,9 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="169" formatCode="0.0000"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <numFmt numFmtId="165" formatCode="0.0000"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
           <color rgb="FF000000"/>
         </left>
@@ -391,6 +417,12 @@
         <bottom style="medium">
           <color rgb="FF000000"/>
         </bottom>
+        <vertical style="medium">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="medium">
+          <color rgb="FF000000"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -410,9 +442,9 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="169" formatCode="0.0000"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <numFmt numFmtId="165" formatCode="0.0000"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
           <color rgb="FF000000"/>
         </left>
@@ -425,6 +457,12 @@
         <bottom style="medium">
           <color rgb="FF000000"/>
         </bottom>
+        <vertical style="medium">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="medium">
+          <color rgb="FF000000"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -445,8 +483,8 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
           <color rgb="FF000000"/>
         </left>
@@ -459,6 +497,12 @@
         <bottom style="medium">
           <color rgb="FF000000"/>
         </bottom>
+        <vertical style="medium">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="medium">
+          <color rgb="FF000000"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -479,8 +523,8 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
           <color rgb="FF000000"/>
         </left>
@@ -493,6 +537,12 @@
         <bottom style="medium">
           <color rgb="FF000000"/>
         </bottom>
+        <vertical style="medium">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="medium">
+          <color rgb="FF000000"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -512,9 +562,9 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="168" formatCode="0.00000"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <numFmt numFmtId="164" formatCode="0.00000"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="medium">
           <color rgb="FF000000"/>
@@ -522,40 +572,54 @@
         <top style="medium">
           <color rgb="FF000000"/>
         </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical style="medium">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="medium">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="medium">
+          <color rgb="FF000000"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
         <bottom style="medium">
           <color rgb="FF000000"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
         <top style="medium">
           <color rgb="FF000000"/>
         </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <bottom style="medium">
           <color rgb="FF000000"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="medium">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="medium">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="medium">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
+      <font>
+        <b val="0"/>
+        <family val="2"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.00000"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -571,18 +635,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{330C9B7C-9DEC-4A55-94BB-E9834BD959C0}" name="Table1" displayName="Table1" ref="A1:F9" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="9" tableBorderDxfId="10" totalsRowBorderDxfId="8">
-  <autoFilter ref="A1:F9" xr:uid="{330C9B7C-9DEC-4A55-94BB-E9834BD959C0}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F9">
-    <sortCondition ref="D1:D9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{330C9B7C-9DEC-4A55-94BB-E9834BD959C0}" name="Table1" displayName="Table1" ref="A1:F14" totalsRowShown="0" headerRowDxfId="0" dataDxfId="10" headerRowBorderDxfId="8" tableBorderDxfId="9" totalsRowBorderDxfId="7">
+  <autoFilter ref="A1:F14" xr:uid="{330C9B7C-9DEC-4A55-94BB-E9834BD959C0}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F14">
+    <sortCondition ref="D1:D14"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{8AF7F365-A0DE-43C4-A2D5-69FA2C8A6F28}" name="Model Name" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{EEBBD775-E053-4374-9CF8-B3642DF18ADE}" name="Batch Size" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{497D6176-C72C-49B7-92E8-9AEA31E178F1}" name="Epoch" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{1F873F5F-4442-4BB1-B82E-6B0D2F5DBE7A}" name="MSE" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{1904A9EC-870C-4009-9595-8123616F356A}" name="MAE" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{9CC926B9-B497-44F3-9E24-C58867CB7942}" name="MPE" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{8AF7F365-A0DE-43C4-A2D5-69FA2C8A6F28}" name="Model Name" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{EEBBD775-E053-4374-9CF8-B3642DF18ADE}" name="Batch Size" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{497D6176-C72C-49B7-92E8-9AEA31E178F1}" name="Epoch" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{1F873F5F-4442-4BB1-B82E-6B0D2F5DBE7A}" name="MSE" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{1904A9EC-870C-4009-9595-8123616F356A}" name="MAE" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{9CC926B9-B497-44F3-9E24-C58867CB7942}" name="MPE" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -885,10 +949,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E4C1E1F-FF86-41D2-98E4-FD2A8E68D35D}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -901,182 +965,282 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="43.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="2" spans="1:6" ht="143.75" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="5">
+        <v>32</v>
+      </c>
+      <c r="C2" s="5">
+        <v>20</v>
+      </c>
+      <c r="D2" s="14">
+        <v>0.46709674600000001</v>
+      </c>
+      <c r="E2" s="14">
+        <v>0.54570943100000002</v>
+      </c>
+      <c r="F2" s="15">
+        <v>15.575237270000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B3" s="5">
         <v>32</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C3" s="5">
         <v>20</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D3" s="6">
         <v>0.49398700000000001</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E3" s="6">
         <v>0.56537300000000001</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F3" s="7">
         <v>15.810715</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="72" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="1">
+    <row r="4" spans="1:6" ht="101" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="A4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="5">
         <v>32</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C4" s="5">
+        <v>8</v>
+      </c>
+      <c r="D4" s="14">
+        <v>0.50310617685317904</v>
+      </c>
+      <c r="E4" s="14">
+        <v>0.566886126995086</v>
+      </c>
+      <c r="F4" s="15">
+        <v>16.075475692748999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="72.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="A5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="5">
+        <v>32</v>
+      </c>
+      <c r="C5" s="5">
         <v>20</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D5" s="8">
         <v>0.51519999999999999</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E5" s="8">
         <v>0.57789999999999997</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F5" s="9">
         <v>16.298300000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A4" s="4" t="s">
+    <row r="6" spans="1:6" ht="101" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="A6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="5">
+        <v>32</v>
+      </c>
+      <c r="C6" s="5">
         <v>8</v>
       </c>
-      <c r="B4" s="1">
-        <v>75</v>
-      </c>
-      <c r="C4" s="1">
+      <c r="D6" s="14">
+        <v>0.53339350223541204</v>
+      </c>
+      <c r="E6" s="14">
+        <v>0.57539176940917902</v>
+      </c>
+      <c r="F6" s="15">
+        <v>16.179872512817301</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="101" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="A7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="5">
         <v>32</v>
       </c>
-      <c r="D4" s="2">
-        <v>0.63270777499999997</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0.636956513</v>
-      </c>
-      <c r="F4" s="5">
-        <v>18.142898559999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1">
-        <v>32</v>
-      </c>
-      <c r="C5" s="1">
+      <c r="C7" s="5">
         <v>20</v>
       </c>
-      <c r="D5" s="2">
-        <v>0.68537431999999998</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0.65762138400000003</v>
-      </c>
-      <c r="F5" s="5">
-        <v>17.496559139999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="1">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1">
-        <v>100</v>
-      </c>
-      <c r="D6" s="3">
-        <v>0.7157</v>
-      </c>
-      <c r="E6" s="3">
-        <v>0.6653</v>
-      </c>
-      <c r="F6" s="6">
-        <v>18.3475</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="1">
-        <v>10</v>
-      </c>
-      <c r="C7" s="1">
-        <v>75</v>
-      </c>
-      <c r="D7" s="2">
-        <v>1.259134293</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0.93609070800000005</v>
-      </c>
-      <c r="F7" s="5">
-        <v>28.3303051</v>
+      <c r="D7" s="8">
+        <v>0.539692282676696</v>
+      </c>
+      <c r="E7" s="14">
+        <v>0.57134431600570601</v>
+      </c>
+      <c r="F7" s="15">
+        <v>16.014867782592699</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="5">
+        <v>75</v>
+      </c>
+      <c r="C8" s="5">
+        <v>32</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0.63270777499999997</v>
+      </c>
+      <c r="E8" s="6">
+        <v>0.636956513</v>
+      </c>
+      <c r="F8" s="7">
+        <v>18.142898559999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="A9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="5">
+        <v>32</v>
+      </c>
+      <c r="C9" s="5">
+        <v>20</v>
+      </c>
+      <c r="D9" s="6">
+        <v>0.68537431999999998</v>
+      </c>
+      <c r="E9" s="6">
+        <v>0.65762138400000003</v>
+      </c>
+      <c r="F9" s="7">
+        <v>17.496559139999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="101" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="A10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="5">
+        <v>32</v>
+      </c>
+      <c r="C10" s="5">
+        <v>20</v>
+      </c>
+      <c r="D10" s="14">
+        <v>0.69350767135620095</v>
+      </c>
+      <c r="E10" s="14">
+        <v>0.66982841491699197</v>
+      </c>
+      <c r="F10" s="15">
+        <v>18.773012161254801</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="A11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5">
+        <v>5</v>
+      </c>
+      <c r="C11" s="5">
+        <v>100</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0.7157</v>
+      </c>
+      <c r="E11" s="8">
+        <v>0.6653</v>
+      </c>
+      <c r="F11" s="9">
+        <v>18.3475</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="29.75" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="A12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="5">
+        <v>10</v>
+      </c>
+      <c r="C12" s="5">
+        <v>75</v>
+      </c>
+      <c r="D12" s="6">
+        <v>1.259134293</v>
+      </c>
+      <c r="E12" s="6">
+        <v>0.93609070800000005</v>
+      </c>
+      <c r="F12" s="7">
+        <v>28.3303051</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="A13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="5">
+        <v>32</v>
+      </c>
+      <c r="C13" s="5">
+        <v>100</v>
+      </c>
+      <c r="D13" s="8">
+        <v>1.26832699775695</v>
+      </c>
+      <c r="E13" s="8">
+        <v>0.93750673532485895</v>
+      </c>
+      <c r="F13" s="9">
+        <v>28.6094245910644</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A14" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B14" s="11">
         <v>32</v>
       </c>
-      <c r="C8" s="1">
-        <v>100</v>
-      </c>
-      <c r="D8" s="3">
-        <v>1.26832699775695</v>
-      </c>
-      <c r="E8" s="3">
-        <v>0.93750673532485895</v>
-      </c>
-      <c r="F8" s="6">
-        <v>28.6094245910644</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.75">
-      <c r="A9" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="8">
-        <v>32</v>
-      </c>
-      <c r="C9" s="8">
+      <c r="C14" s="11">
         <v>20</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D14" s="12">
         <v>1.3218526840209901</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E14" s="12">
         <v>0.94115793704986495</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F14" s="13">
         <v>28.0158367156982</v>
       </c>
     </row>

</xml_diff>